<commit_message>
added signal names, circuit representation, piloting from circuit, updated files to deploy and doc
</commit_message>
<xml_diff>
--- a/Docs/Creating setup file.xlsx
+++ b/Docs/Creating setup file.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="73">
   <si>
     <t>Nombre de signaux</t>
   </si>
@@ -179,6 +179,66 @@
   </si>
   <si>
     <t>Key234</t>
+  </si>
+  <si>
+    <t>Signal 1</t>
+  </si>
+  <si>
+    <t>Signal 2</t>
+  </si>
+  <si>
+    <t>Signal 3</t>
+  </si>
+  <si>
+    <t>Signal 4</t>
+  </si>
+  <si>
+    <t>Signal 5</t>
+  </si>
+  <si>
+    <t>Signal 6</t>
+  </si>
+  <si>
+    <t>Signal 7</t>
+  </si>
+  <si>
+    <t>Signal 8</t>
+  </si>
+  <si>
+    <t>cote gauceh</t>
+  </si>
+  <si>
+    <t>milieu</t>
+  </si>
+  <si>
+    <t>haut</t>
+  </si>
+  <si>
+    <t>bas</t>
+  </si>
+  <si>
+    <t>par ici</t>
+  </si>
+  <si>
+    <t>par la</t>
+  </si>
+  <si>
+    <t>par la bas</t>
+  </si>
+  <si>
+    <t>tut en haut</t>
+  </si>
+  <si>
+    <t>Signal</t>
+  </si>
+  <si>
+    <t>Total Signal</t>
+  </si>
+  <si>
+    <t>Name Signal</t>
+  </si>
+  <si>
+    <t>sna</t>
   </si>
 </sst>
 </file>
@@ -583,10 +643,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -600,8 +660,8 @@
         <v>35</v>
       </c>
       <c r="B1" s="2" t="str">
-        <f>Variables!B12</f>
-        <v>?nsi=8&amp;nai=8&amp;ntr=4&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;sec=Key234</v>
+        <f>Variables!B13</f>
+        <v>?nsi=8&amp;nai=8&amp;ntr=4&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;sna1=cote gauceh&amp;spl1=200&amp;spt1=550&amp;sna2=milieu&amp;spl2=120&amp;spt2=10&amp;sna3=haut&amp;spl3=279&amp;spt3=523&amp;sna4=bas&amp;spl4=250&amp;spt4=160&amp;sna5=par ici&amp;spl5=130&amp;spt5=160&amp;sna6=par la&amp;spl6=33&amp;spt6=645&amp;sna7=par la bas&amp;spl7=127&amp;spt7=457&amp;sna8=tut en haut&amp;spl8=536&amp;spt8=546&amp;sec=Key234</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -842,6 +902,130 @@
       </c>
       <c r="D24" s="5">
         <v>566</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A25" s="1"/>
+      <c r="B25" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="C25" s="6" t="s">
+        <v>49</v>
+      </c>
+      <c r="D25" s="6" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" t="s">
+        <v>61</v>
+      </c>
+      <c r="C26" s="5">
+        <v>200</v>
+      </c>
+      <c r="D26" s="5">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A27" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B27" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="5">
+        <v>120</v>
+      </c>
+      <c r="D27" s="5">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A28" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="B28" t="s">
+        <v>63</v>
+      </c>
+      <c r="C28" s="5">
+        <v>279</v>
+      </c>
+      <c r="D28" s="5">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A29" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="B29" t="s">
+        <v>64</v>
+      </c>
+      <c r="C29" s="5">
+        <v>250</v>
+      </c>
+      <c r="D29" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" t="s">
+        <v>65</v>
+      </c>
+      <c r="C30" s="5">
+        <v>130</v>
+      </c>
+      <c r="D30" s="5">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A31" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B31" t="s">
+        <v>66</v>
+      </c>
+      <c r="C31" s="5">
+        <v>33</v>
+      </c>
+      <c r="D31" s="5">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A32" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B32" t="s">
+        <v>67</v>
+      </c>
+      <c r="C32" s="5">
+        <v>127</v>
+      </c>
+      <c r="D32" s="5">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B33" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="5">
+        <v>536</v>
+      </c>
+      <c r="D33" s="5">
+        <v>546</v>
       </c>
     </row>
   </sheetData>
@@ -870,10 +1054,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:B29"/>
+  <dimension ref="A3:B40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -945,159 +1129,253 @@
         <v>30</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>18</v>
-      </c>
-      <c r="B12" t="str">
-        <f>B13&amp;B19&amp;B29&amp;Variables!B9&amp;"="&amp;Paramétrage!B8</f>
-        <v>?nsi=8&amp;nai=8&amp;ntr=4&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;sec=Key234</v>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
+        <v>18</v>
+      </c>
+      <c r="B13" t="str">
+        <f>B14&amp;B20&amp;B30&amp;B40&amp;Variables!B9&amp;"="&amp;Paramétrage!B8</f>
+        <v>?nsi=8&amp;nai=8&amp;ntr=4&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;sna1=cote gauceh&amp;spl1=200&amp;spt1=550&amp;sna2=milieu&amp;spl2=120&amp;spt2=10&amp;sna3=haut&amp;spl3=279&amp;spt3=523&amp;sna4=bas&amp;spl4=250&amp;spt4=160&amp;sna5=par ici&amp;spl5=130&amp;spt5=160&amp;sna6=par la&amp;spl6=33&amp;spt6=645&amp;sna7=par la bas&amp;spl7=127&amp;spt7=457&amp;sna8=tut en haut&amp;spl8=536&amp;spt8=546&amp;sec=Key234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B13" s="2" t="str">
+      <c r="B14" s="2" t="str">
         <f>"?"&amp;Variables!B3&amp;"="&amp;Paramétrage!B5&amp;"&amp;"&amp;Variables!B4&amp;"="&amp;Paramétrage!B6&amp;"&amp;"&amp;Variables!B5&amp;"="&amp;Paramétrage!B7</f>
         <v>?nsi=8&amp;nai=8&amp;ntr=4</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
         <v>17</v>
       </c>
-      <c r="B14" s="2"/>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A15">
-        <v>1</v>
-      </c>
-      <c r="B15" t="str">
-        <f>IF(Paramétrage!B11&lt;&gt;"",$B$7&amp;A15&amp;"="&amp;Paramétrage!B11&amp;"&amp;"&amp;$B$6&amp;A15&amp;"="&amp;Paramétrage!D11&amp;"&amp;"&amp;$B$8&amp;A15&amp;"="&amp;Paramétrage!C11&amp;"&amp;","")</f>
-        <v>tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;</v>
-      </c>
+      <c r="B15" s="2"/>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B16" t="str">
-        <f>IF(Paramétrage!B12&lt;&gt;"",$B$7&amp;A16&amp;"="&amp;Paramétrage!B12&amp;"&amp;"&amp;$B$6&amp;A16&amp;"="&amp;Paramétrage!D12&amp;"&amp;"&amp;$B$8&amp;A16&amp;"="&amp;Paramétrage!C12&amp;"&amp;","")</f>
-        <v>tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;</v>
+        <f>IF(Paramétrage!B11&lt;&gt;"",$B$7&amp;A16&amp;"="&amp;Paramétrage!B11&amp;"&amp;"&amp;$B$6&amp;A16&amp;"="&amp;Paramétrage!D11&amp;"&amp;"&amp;$B$8&amp;A16&amp;"="&amp;Paramétrage!C11&amp;"&amp;","")</f>
+        <v>tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B17" t="str">
-        <f>IF(Paramétrage!B13&lt;&gt;"",$B$7&amp;A17&amp;"="&amp;Paramétrage!B13&amp;"&amp;"&amp;$B$6&amp;A17&amp;"="&amp;Paramétrage!D13&amp;"&amp;"&amp;$B$8&amp;A17&amp;"="&amp;Paramétrage!C13&amp;"&amp;","")</f>
-        <v>tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;</v>
+        <f>IF(Paramétrage!B12&lt;&gt;"",$B$7&amp;A17&amp;"="&amp;Paramétrage!B12&amp;"&amp;"&amp;$B$6&amp;A17&amp;"="&amp;Paramétrage!D12&amp;"&amp;"&amp;$B$8&amp;A17&amp;"="&amp;Paramétrage!C12&amp;"&amp;","")</f>
+        <v>tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
+        <v>3</v>
+      </c>
+      <c r="B18" t="str">
+        <f>IF(Paramétrage!B13&lt;&gt;"",$B$7&amp;A18&amp;"="&amp;Paramétrage!B13&amp;"&amp;"&amp;$B$6&amp;A18&amp;"="&amp;Paramétrage!D13&amp;"&amp;"&amp;$B$8&amp;A18&amp;"="&amp;Paramétrage!C13&amp;"&amp;","")</f>
+        <v>tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19">
         <v>4</v>
       </c>
-      <c r="B18" t="str">
-        <f>IF(Paramétrage!B14&lt;&gt;"",$B$7&amp;A18&amp;"="&amp;Paramétrage!B14&amp;"&amp;"&amp;$B$6&amp;A18&amp;"="&amp;Paramétrage!D14&amp;"&amp;"&amp;$B$8&amp;A18&amp;"="&amp;Paramétrage!C14&amp;"&amp;","")</f>
+      <c r="B19" t="str">
+        <f>IF(Paramétrage!B14&lt;&gt;"",$B$7&amp;A19&amp;"="&amp;Paramétrage!B14&amp;"&amp;"&amp;$B$6&amp;A19&amp;"="&amp;Paramétrage!D14&amp;"&amp;"&amp;$B$8&amp;A19&amp;"="&amp;Paramétrage!C14&amp;"&amp;","")</f>
         <v>tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>17</v>
-      </c>
-      <c r="B19" t="str">
-        <f>"&amp;"&amp;B15&amp;B16&amp;B17&amp;B18</f>
-        <v>&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="str">
+        <f>"&amp;"&amp;B16&amp;B17&amp;B18&amp;B19</f>
+        <v>&amp;tc1=1&amp;tn1=Marchandise rouge&amp;tv1=5&amp;tc2=1&amp;tn2=Passager rouge&amp;tv2=5&amp;tc3=2&amp;tn3=Marchandise jaune 1&amp;tv3=5&amp;tc4=2&amp;tn4=Marchandise jaune 2&amp;tv4=5&amp;</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
         <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A21">
-        <v>1</v>
-      </c>
-      <c r="B21" t="str">
-        <f>$B$10&amp;Variables!A21&amp;"="&amp;Paramétrage!B17&amp;"&amp;"&amp;"pl"&amp;A21&amp;"="&amp;Paramétrage!C17&amp;"&amp;pt"&amp;A21&amp;"="&amp;Paramétrage!D17&amp;"&amp;"</f>
-        <v>ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B22" t="str">
-        <f>$B$10&amp;Variables!A22&amp;"="&amp;Paramétrage!B18&amp;"&amp;"&amp;"pl"&amp;A22&amp;"="&amp;Paramétrage!C18&amp;"&amp;pt"&amp;A22&amp;"="&amp;Paramétrage!D18&amp;"&amp;"</f>
-        <v>ain2=Grue&amp;pl2=140&amp;pt2=30&amp;</v>
+        <f>$B$10&amp;Variables!A22&amp;"="&amp;Paramétrage!B17&amp;"&amp;"&amp;"pl"&amp;A22&amp;"="&amp;Paramétrage!C17&amp;"&amp;pt"&amp;A22&amp;"="&amp;Paramétrage!D17&amp;"&amp;"</f>
+        <v>ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B23" t="str">
-        <f>$B$10&amp;Variables!A23&amp;"="&amp;Paramétrage!B19&amp;"&amp;"&amp;"pl"&amp;A23&amp;"="&amp;Paramétrage!C19&amp;"&amp;pt"&amp;A23&amp;"="&amp;Paramétrage!D19&amp;"&amp;"</f>
-        <v>ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;</v>
+        <f>$B$10&amp;Variables!A23&amp;"="&amp;Paramétrage!B18&amp;"&amp;"&amp;"pl"&amp;A23&amp;"="&amp;Paramétrage!C18&amp;"&amp;pt"&amp;A23&amp;"="&amp;Paramétrage!D18&amp;"&amp;"</f>
+        <v>ain2=Grue&amp;pl2=140&amp;pt2=30&amp;</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B24" t="str">
-        <f>$B$10&amp;Variables!A24&amp;"="&amp;Paramétrage!B20&amp;"&amp;"&amp;"pl"&amp;A24&amp;"="&amp;Paramétrage!C20&amp;"&amp;pt"&amp;A24&amp;"="&amp;Paramétrage!D20&amp;"&amp;"</f>
-        <v>ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;</v>
+        <f>$B$10&amp;Variables!A24&amp;"="&amp;Paramétrage!B19&amp;"&amp;"&amp;"pl"&amp;A24&amp;"="&amp;Paramétrage!C19&amp;"&amp;pt"&amp;A24&amp;"="&amp;Paramétrage!D19&amp;"&amp;"</f>
+        <v>ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B25" t="str">
-        <f>$B$10&amp;Variables!A25&amp;"="&amp;Paramétrage!B21&amp;"&amp;"&amp;"pl"&amp;A25&amp;"="&amp;Paramétrage!C21&amp;"&amp;pt"&amp;A25&amp;"="&amp;Paramétrage!D21&amp;"&amp;"</f>
-        <v>ain5=Depot&amp;pl5=150&amp;pt5=180&amp;</v>
+        <f>$B$10&amp;Variables!A25&amp;"="&amp;Paramétrage!B20&amp;"&amp;"&amp;"pl"&amp;A25&amp;"="&amp;Paramétrage!C20&amp;"&amp;pt"&amp;A25&amp;"="&amp;Paramétrage!D20&amp;"&amp;"</f>
+        <v>ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B26" t="str">
-        <f>$B$10&amp;Variables!A26&amp;"="&amp;Paramétrage!B22&amp;"&amp;"&amp;"pl"&amp;A26&amp;"="&amp;Paramétrage!D22&amp;"&amp;pt"&amp;A26&amp;"="&amp;Paramétrage!C22&amp;"&amp;"</f>
-        <v>ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;</v>
+        <f>$B$10&amp;Variables!A26&amp;"="&amp;Paramétrage!B21&amp;"&amp;"&amp;"pl"&amp;A26&amp;"="&amp;Paramétrage!C21&amp;"&amp;pt"&amp;A26&amp;"="&amp;Paramétrage!D21&amp;"&amp;"</f>
+        <v>ain5=Depot&amp;pl5=150&amp;pt5=180&amp;</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B27" t="str">
-        <f>$B$10&amp;Variables!A27&amp;"="&amp;Paramétrage!B23&amp;"&amp;"&amp;"pl"&amp;A27&amp;"="&amp;Paramétrage!C23&amp;"&amp;pt"&amp;A27&amp;"="&amp;Paramétrage!D23&amp;"&amp;"</f>
-        <v>ain7=Police&amp;pl7=137&amp;pt7=497&amp;</v>
+        <f>$B$10&amp;Variables!A27&amp;"="&amp;Paramétrage!B22&amp;"&amp;"&amp;"pl"&amp;A27&amp;"="&amp;Paramétrage!D22&amp;"&amp;pt"&amp;A27&amp;"="&amp;Paramétrage!C22&amp;"&amp;"</f>
+        <v>ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
+        <v>7</v>
+      </c>
+      <c r="B28" t="str">
+        <f>$B$10&amp;Variables!A28&amp;"="&amp;Paramétrage!B23&amp;"&amp;"&amp;"pl"&amp;A28&amp;"="&amp;Paramétrage!C23&amp;"&amp;pt"&amp;A28&amp;"="&amp;Paramétrage!D23&amp;"&amp;"</f>
+        <v>ain7=Police&amp;pl7=137&amp;pt7=497&amp;</v>
+      </c>
+    </row>
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A29">
         <v>8</v>
       </c>
-      <c r="B28" t="str">
-        <f>$B$10&amp;Variables!A28&amp;"="&amp;Paramétrage!B24&amp;"&amp;"&amp;"pl"&amp;A28&amp;"="&amp;Paramétrage!D24&amp;"&amp;pt"&amp;A28&amp;"="&amp;Paramétrage!C24&amp;"&amp;"</f>
+      <c r="B29" t="str">
+        <f>$B$10&amp;Variables!A29&amp;"="&amp;Paramétrage!B24&amp;"&amp;"&amp;"pl"&amp;A29&amp;"="&amp;Paramétrage!D24&amp;"&amp;pt"&amp;A29&amp;"="&amp;Paramétrage!C24&amp;"&amp;"</f>
         <v>ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>20</v>
       </c>
-      <c r="B29" t="str">
-        <f>B21&amp;B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28</f>
+      <c r="B30" t="str">
+        <f>B22&amp;B23&amp;B24&amp;B25&amp;B26&amp;B27&amp;B28&amp;B29</f>
         <v>ain1=Butte verte&amp;pl1=220&amp;pt1=600&amp;ain2=Grue&amp;pl2=140&amp;pt2=30&amp;ain3=Arbre&amp;pl3=297&amp;pt3=497&amp;ain4=Hobbit&amp;pl4=300&amp;pt4=180&amp;ain5=Depot&amp;pl5=150&amp;pt5=180&amp;ain6=Hobbit&amp;pl6=651&amp;pt6=48&amp;ain7=Police&amp;pl7=137&amp;pt7=497&amp;ain8=Chateau&amp;pl8=566&amp;pt8=556&amp;</v>
+      </c>
+    </row>
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" t="str">
+        <f>$B$11&amp;Variables!A32&amp;"="&amp;Paramétrage!B26&amp;"&amp;"&amp;"spl"&amp;A32&amp;"="&amp;Paramétrage!C26&amp;"&amp;spt"&amp;A32&amp;"="&amp;Paramétrage!D26&amp;"&amp;"</f>
+        <v>sna1=cote gauceh&amp;spl1=200&amp;spt1=550&amp;</v>
+      </c>
+    </row>
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>2</v>
+      </c>
+      <c r="B33" t="str">
+        <f>$B$11&amp;Variables!A33&amp;"="&amp;Paramétrage!B27&amp;"&amp;"&amp;"spl"&amp;A33&amp;"="&amp;Paramétrage!C27&amp;"&amp;spt"&amp;A33&amp;"="&amp;Paramétrage!D27&amp;"&amp;"</f>
+        <v>sna2=milieu&amp;spl2=120&amp;spt2=10&amp;</v>
+      </c>
+    </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>3</v>
+      </c>
+      <c r="B34" t="str">
+        <f>$B$11&amp;Variables!A34&amp;"="&amp;Paramétrage!B28&amp;"&amp;"&amp;"spl"&amp;A34&amp;"="&amp;Paramétrage!C28&amp;"&amp;spt"&amp;A34&amp;"="&amp;Paramétrage!D28&amp;"&amp;"</f>
+        <v>sna3=haut&amp;spl3=279&amp;spt3=523&amp;</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>4</v>
+      </c>
+      <c r="B35" t="str">
+        <f>$B$11&amp;Variables!A35&amp;"="&amp;Paramétrage!B29&amp;"&amp;"&amp;"spl"&amp;A35&amp;"="&amp;Paramétrage!C29&amp;"&amp;spt"&amp;A35&amp;"="&amp;Paramétrage!D29&amp;"&amp;"</f>
+        <v>sna4=bas&amp;spl4=250&amp;spt4=160&amp;</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A36">
+        <v>5</v>
+      </c>
+      <c r="B36" t="str">
+        <f>$B$11&amp;Variables!A36&amp;"="&amp;Paramétrage!B30&amp;"&amp;"&amp;"spl"&amp;A36&amp;"="&amp;Paramétrage!C30&amp;"&amp;spt"&amp;A36&amp;"="&amp;Paramétrage!D30&amp;"&amp;"</f>
+        <v>sna5=par ici&amp;spl5=130&amp;spt5=160&amp;</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A37">
+        <v>6</v>
+      </c>
+      <c r="B37" t="str">
+        <f>$B$11&amp;Variables!A37&amp;"="&amp;Paramétrage!B31&amp;"&amp;"&amp;"spl"&amp;A37&amp;"="&amp;Paramétrage!C31&amp;"&amp;spt"&amp;A37&amp;"="&amp;Paramétrage!D31&amp;"&amp;"</f>
+        <v>sna6=par la&amp;spl6=33&amp;spt6=645&amp;</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A38">
+        <v>7</v>
+      </c>
+      <c r="B38" t="str">
+        <f>$B$11&amp;Variables!A38&amp;"="&amp;Paramétrage!B32&amp;"&amp;"&amp;"spl"&amp;A38&amp;"="&amp;Paramétrage!C32&amp;"&amp;spt"&amp;A38&amp;"="&amp;Paramétrage!D32&amp;"&amp;"</f>
+        <v>sna7=par la bas&amp;spl7=127&amp;spt7=457&amp;</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A39">
+        <v>8</v>
+      </c>
+      <c r="B39" t="str">
+        <f>$B$11&amp;Variables!A39&amp;"="&amp;Paramétrage!B33&amp;"&amp;"&amp;"spl"&amp;A39&amp;"="&amp;Paramétrage!C33&amp;"&amp;spt"&amp;A39&amp;"="&amp;Paramétrage!D33&amp;"&amp;"</f>
+        <v>sna8=tut en haut&amp;spl8=536&amp;spt8=546&amp;</v>
+      </c>
+    </row>
+    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>70</v>
+      </c>
+      <c r="B40" t="str">
+        <f>B32&amp;B33&amp;B34&amp;B35&amp;B36&amp;B37&amp;B38&amp;B39</f>
+        <v>sna1=cote gauceh&amp;spl1=200&amp;spt1=550&amp;sna2=milieu&amp;spl2=120&amp;spt2=10&amp;sna3=haut&amp;spl3=279&amp;spt3=523&amp;sna4=bas&amp;spl4=250&amp;spt4=160&amp;sna5=par ici&amp;spl5=130&amp;spt5=160&amp;sna6=par la&amp;spl6=33&amp;spt6=645&amp;sna7=par la bas&amp;spl7=127&amp;spt7=457&amp;sna8=tut en haut&amp;spl8=536&amp;spt8=546&amp;</v>
       </c>
     </row>
   </sheetData>

</xml_diff>